<commit_message>
Add positional force to group nodes categorically
</commit_message>
<xml_diff>
--- a/network.xlsx
+++ b/network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akokai/Documents/ESPM/KCGC Project/safer-chemicals-network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C37BBDB-4566-4F48-AB14-5E5EA1A9EF13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0400D6-DF8A-7F45-9045-0506AC3FBBAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11320" yWindow="4960" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>Akos Kokai</author>
   </authors>
   <commentList>
-    <comment ref="H27" authorId="0" shapeId="0" xr:uid="{B22F9111-4A1E-D34D-9C52-DB1E0DCE8972}">
+    <comment ref="H29" authorId="0" shapeId="0" xr:uid="{B22F9111-4A1E-D34D-9C52-DB1E0DCE8972}">
       <text>
         <r>
           <rPr>
@@ -64,14 +64,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="108">
   <si>
     <t>label</t>
   </si>
   <si>
-    <t>sector</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
@@ -141,18 +138,6 @@
     <t>Pharos</t>
   </si>
   <si>
-    <t>Maine: Safer Chemicals in Children's Products Rules</t>
-  </si>
-  <si>
-    <t>USA/ME Safer Chemicals</t>
-  </si>
-  <si>
-    <t>USA/CA Safer Consumer Products</t>
-  </si>
-  <si>
-    <t>USA/WA SB 5181</t>
-  </si>
-  <si>
     <t>SUBSPORT</t>
   </si>
   <si>
@@ -165,18 +150,9 @@
     <t>Chemicals</t>
   </si>
   <si>
-    <t>https://app.leg.wa.gov/billsummary?BillNumber=5181&amp;Chamber=Senate&amp;Year=2013</t>
-  </si>
-  <si>
-    <t>The bill didn't pass</t>
-  </si>
-  <si>
     <t>https://www.greenscreenchemicals.org/learn/full-greenscreen-method</t>
   </si>
   <si>
-    <t>Alternatives Analysis Guide</t>
-  </si>
-  <si>
     <t>Chemical Hazard Data Commons</t>
   </si>
   <si>
@@ -186,9 +162,6 @@
     <t>GHS</t>
   </si>
   <si>
-    <t>Safer Choice Standard</t>
-  </si>
-  <si>
     <t>https://www.epa.gov/saferchoice/standard</t>
   </si>
   <si>
@@ -198,9 +171,6 @@
     <t>TCO Certified requires the use of GreenScreen to assess some […] chemicals for a required credit.</t>
   </si>
   <si>
-    <t>GreenScreen uses technical criteria, metrics, and thresholds for hazard classification from GHS.</t>
-  </si>
-  <si>
     <t>GreenScreen uses hazard endpoint definitions, the low/medium/high endpoint hazard level scheme, and also technical criteria and metrics for hazard classification from Safer Choice.</t>
   </si>
   <si>
@@ -231,12 +201,6 @@
     <t>ChemSec Marketplace</t>
   </si>
   <si>
-    <t>nodetype</t>
-  </si>
-  <si>
-    <t>collection</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -282,9 +246,6 @@
     <t>The Interstate Chemical Clearinghouse (IC2) Chemical Hazard Assessment Database enables users to search for GreenScreen and Quick Chemical Assessment Tool (QCAT) assessments.</t>
   </si>
   <si>
-    <t>IC2 AA Guide</t>
-  </si>
-  <si>
     <t>The IC2 Alternatives Assessment guide references the GreenScreen method as the preferred form of evaluation for the Hazard module.</t>
   </si>
   <si>
@@ -294,18 +255,12 @@
     <t>https://www.nap.edu/catalog/18872/a-framework-to-guide-selection-of-chemical-alternatives</t>
   </si>
   <si>
-    <t>NRC Framework Guide</t>
-  </si>
-  <si>
     <t>NRC Framework to Guide Selection of Chemical Alternatives</t>
   </si>
   <si>
     <t>The NRC Framework Guide references the GreenScreen method as an applicable tool for hazard assessment within the frameworks of alternatives assessment.</t>
   </si>
   <si>
-    <t>BizNGO AA Protocol</t>
-  </si>
-  <si>
     <t>https://www.bizngo.org/alternatives-assessment/chemical-alternatives-assessment-protocol</t>
   </si>
   <si>
@@ -328,6 +283,111 @@
   </si>
   <si>
     <t>QCAT is based on a simplified version of the GreenScreen framework.</t>
+  </si>
+  <si>
+    <t>GreenScreen Certified for Building Products</t>
+  </si>
+  <si>
+    <t>C2C</t>
+  </si>
+  <si>
+    <t>Safer Choice</t>
+  </si>
+  <si>
+    <t>GSC-BP</t>
+  </si>
+  <si>
+    <t>GSC</t>
+  </si>
+  <si>
+    <t>Levis Screened Chemistry</t>
+  </si>
+  <si>
+    <t>Levis</t>
+  </si>
+  <si>
+    <t>ILFI LPC</t>
+  </si>
+  <si>
+    <t>Living Product Challenge</t>
+  </si>
+  <si>
+    <t>"GS is used to develop the acceptable lists for FRs and phthalates"</t>
+  </si>
+  <si>
+    <t>GreenScreen uses definitions, technical criteria, metrics, and thresholds for hazard classification derived from GHS.</t>
+  </si>
+  <si>
+    <t>Safer Choice uses definitions, technical criteria, metrics, and thresholds for hazard classification derived from GHS.</t>
+  </si>
+  <si>
+    <t>The C2C Material Health Assessment methodology uses definitions, technical criteria, metrics, and thresholds for hazard classification derived from GHS.</t>
+  </si>
+  <si>
+    <t>Certified GreenScreen assessments may be used as sources of information for conducting C2C Material Health Assessments.</t>
+  </si>
+  <si>
+    <t>GreenScreen uses technical criteria, metrics, and thresholds for hazard classification derived from the Safer Choice Standard.</t>
+  </si>
+  <si>
+    <t>DTSC AA</t>
+  </si>
+  <si>
+    <t>Maine (US) Safer Chemicals in Children's Products Rules</t>
+  </si>
+  <si>
+    <t>Maine's Safer Chemicals in Children's Products Rules</t>
+  </si>
+  <si>
+    <t>WA PBDE Law</t>
+  </si>
+  <si>
+    <t>Maine SCCP</t>
+  </si>
+  <si>
+    <t>Cradle-to-Cradle Certified</t>
+  </si>
+  <si>
+    <t>ZDHC</t>
+  </si>
+  <si>
+    <t>Data Commons</t>
+  </si>
+  <si>
+    <t>Marketplace</t>
+  </si>
+  <si>
+    <t>BizNGO AA</t>
+  </si>
+  <si>
+    <t>NRC AA</t>
+  </si>
+  <si>
+    <t>IC2 Alternatives Assessment Guide</t>
+  </si>
+  <si>
+    <t>IC2 AA</t>
+  </si>
+  <si>
+    <t>Alternatives Assessment</t>
+  </si>
+  <si>
+    <t>Hazard Assessment</t>
+  </si>
+  <si>
+    <t>Green Design</t>
+  </si>
+  <si>
+    <t>Fill in from GS origin story</t>
+  </si>
+  <si>
+    <t>Resource Type</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Topic</t>
   </si>
 </sst>
 </file>
@@ -840,7 +900,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
@@ -853,6 +913,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1209,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,28 +1286,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1252,25 +1315,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1278,23 +1341,23 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1302,74 +1365,72 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1377,22 +1438,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>103</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1400,22 +1464,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1423,22 +1487,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1446,22 +1510,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1469,22 +1533,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1492,22 +1556,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1515,25 +1579,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1541,22 +1602,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="G14" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1564,22 +1625,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>103</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1587,48 +1651,45 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1636,45 +1697,48 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>102</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1682,22 +1746,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="G20" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1705,22 +1769,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
         <v>27</v>
       </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1728,22 +1792,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1751,25 +1815,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="G23" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1777,22 +1838,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" t="s">
-        <v>67</v>
+        <v>102</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1800,128 +1861,196 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="G25" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G26" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="G27" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>86</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" t="s">
+        <v>66</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" t="s">
+        <v>81</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1" xr:uid="{B31F22F4-A4A7-3C45-B76E-9EA4FEEE6A48}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{8C6A6C3C-4D8C-634A-8A8E-F2F3BCDEC592}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{34B08EC6-6F1D-FC44-8984-2BA436B68885}"/>
-    <hyperlink ref="F13" r:id="rId4" xr:uid="{D0B0FB0C-1609-6640-BE12-83379742761F}"/>
-    <hyperlink ref="F17" r:id="rId5" xr:uid="{A7094861-EBE0-214D-8880-0212926E7044}"/>
-    <hyperlink ref="F25" r:id="rId6" xr:uid="{D50C0172-84BE-984E-BE0E-252D3E379FC0}"/>
-    <hyperlink ref="F26" r:id="rId7" xr:uid="{67CA9918-B934-9F4F-8084-670BE7972AE3}"/>
-    <hyperlink ref="F27" r:id="rId8" xr:uid="{6B1CD0A7-2DBE-C348-B00A-C9912AFFE684}"/>
-    <hyperlink ref="F28" r:id="rId9" xr:uid="{702321C8-4D2B-1245-A359-A3EBE4673414}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{8C6A6C3C-4D8C-634A-8A8E-F2F3BCDEC592}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{34B08EC6-6F1D-FC44-8984-2BA436B68885}"/>
+    <hyperlink ref="F15" r:id="rId3" xr:uid="{D0B0FB0C-1609-6640-BE12-83379742761F}"/>
+    <hyperlink ref="F19" r:id="rId4" xr:uid="{A7094861-EBE0-214D-8880-0212926E7044}"/>
+    <hyperlink ref="F27" r:id="rId5" xr:uid="{D50C0172-84BE-984E-BE0E-252D3E379FC0}"/>
+    <hyperlink ref="F28" r:id="rId6" xr:uid="{67CA9918-B934-9F4F-8084-670BE7972AE3}"/>
+    <hyperlink ref="F29" r:id="rId7" xr:uid="{6B1CD0A7-2DBE-C348-B00A-C9912AFFE684}"/>
+    <hyperlink ref="F26" r:id="rId8" xr:uid="{702321C8-4D2B-1245-A359-A3EBE4673414}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId10"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1930,24 +2059,24 @@
     <col min="4" max="5" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1955,7 +2084,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="D2" t="str">
         <f>VLOOKUP(A2, nodes!A:B, 2)</f>
@@ -1966,7 +2095,7 @@
         <v>GHS</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1974,7 +2103,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="D3" t="str">
         <f>VLOOKUP(A3, nodes!A:B, 2)</f>
@@ -1982,220 +2111,235 @@
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(B3, nodes!A:B, 2)</f>
-        <v>Safer Choice Standard</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>Safer Choice</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="D4" t="str">
         <f>VLOOKUP(A4, nodes!A:B, 2)</f>
-        <v>HPD</v>
+        <v>Safer Choice</v>
       </c>
       <c r="E4" t="str">
         <f>VLOOKUP(B4, nodes!A:B, 2)</f>
-        <v>GreenScreen</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>GHS</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D5" t="str">
         <f>VLOOKUP(A5, nodes!A:B, 2)</f>
-        <v>LEED</v>
+        <v>C2C</v>
       </c>
       <c r="E5" t="str">
         <f>VLOOKUP(B5, nodes!A:B, 2)</f>
-        <v>GreenScreen</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>GHS</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="D6" t="str">
         <f>VLOOKUP(A6, nodes!A:B, 2)</f>
-        <v>BIFMA e3</v>
+        <v>C2C</v>
       </c>
       <c r="E6" t="str">
         <f>VLOOKUP(B6, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D7" t="str">
         <f>VLOOKUP(A7, nodes!A:B, 2)</f>
-        <v>BIFMA LEVEL</v>
+        <v>GreenScreen</v>
       </c>
       <c r="E7" t="str">
         <f>VLOOKUP(B7, nodes!A:B, 2)</f>
-        <v>GreenScreen</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>Safer Choice</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>0</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D8" t="str">
         <f>VLOOKUP(A8, nodes!A:B, 2)</f>
-        <v>EPEAT</v>
+        <v>HPD</v>
       </c>
       <c r="E8" t="str">
         <f>VLOOKUP(B8, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>43</v>
+      <c r="C9" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D9" t="str">
         <f>VLOOKUP(A9, nodes!A:B, 2)</f>
-        <v>TCO Certified</v>
+        <v>LEED</v>
       </c>
       <c r="E9" t="str">
         <f>VLOOKUP(B9, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="D10" t="str">
         <f>VLOOKUP(A10, nodes!A:B, 2)</f>
-        <v>GreenScreen Certified</v>
+        <v>BIFMA e3</v>
       </c>
       <c r="E10" t="str">
         <f>VLOOKUP(B10, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="D11" t="str">
         <f>VLOOKUP(A11, nodes!A:B, 2)</f>
-        <v>ZDHC Chemicals Module</v>
+        <v>BIFMA LEVEL</v>
       </c>
       <c r="E11" t="str">
         <f>VLOOKUP(B11, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" t="str">
         <f>VLOOKUP(A12, nodes!A:B, 2)</f>
-        <v>EPA SCIL</v>
+        <v>EPEAT</v>
       </c>
       <c r="E12" t="str">
         <f>VLOOKUP(B12, nodes!A:B, 2)</f>
-        <v>Safer Choice Standard</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>GreenScreen</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>0</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="D13" t="str">
         <f>VLOOKUP(A13, nodes!A:B, 2)</f>
-        <v>Chemical Hazard Data Commons</v>
+        <v>TCO Certified</v>
       </c>
       <c r="E13" t="str">
         <f>VLOOKUP(B13, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="D14" t="str">
         <f>VLOOKUP(A14, nodes!A:B, 2)</f>
-        <v>Pharos</v>
+        <v>GSC</v>
       </c>
       <c r="E14" t="str">
         <f>VLOOKUP(B14, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="D15" t="str">
         <f>VLOOKUP(A15, nodes!A:B, 2)</f>
-        <v>Material Wise</v>
+        <v>GSC-BP</v>
       </c>
       <c r="E15" t="str">
         <f>VLOOKUP(B15, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="D16" t="str">
         <f>VLOOKUP(A16, nodes!A:B, 2)</f>
-        <v>IC2 Database</v>
+        <v>ZDHC</v>
       </c>
       <c r="E16" t="str">
         <f>VLOOKUP(B16, nodes!A:B, 2)</f>
@@ -2204,30 +2348,30 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D17" t="str">
         <f>VLOOKUP(A17, nodes!A:B, 2)</f>
-        <v>IC2 Database</v>
+        <v>EPA SCIL</v>
       </c>
       <c r="E17" t="str">
         <f>VLOOKUP(B17, nodes!A:B, 2)</f>
-        <v>QCAT</v>
+        <v>Safer Choice</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>VLOOKUP(A18, nodes!A:B, 2)</f>
-        <v>SUBSPORT</v>
+        <v>Data Commons</v>
       </c>
       <c r="E18" t="str">
         <f>VLOOKUP(B18, nodes!A:B, 2)</f>
@@ -2236,14 +2380,14 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>VLOOKUP(A19, nodes!A:B, 2)</f>
-        <v>ToxFMD DB</v>
+        <v>Pharos</v>
       </c>
       <c r="E19" t="str">
         <f>VLOOKUP(B19, nodes!A:B, 2)</f>
@@ -2251,15 +2395,15 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
+      <c r="A20" s="7">
+        <v>16</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>VLOOKUP(A20, nodes!A:B, 2)</f>
-        <v>ChemSec Marketplace</v>
+        <v>Material Wise</v>
       </c>
       <c r="E20" t="str">
         <f>VLOOKUP(B20, nodes!A:B, 2)</f>
@@ -2267,31 +2411,31 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
+      <c r="A21" s="7">
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D21" t="str">
         <f>VLOOKUP(A21, nodes!A:B, 2)</f>
-        <v>USA/CA Safer Consumer Products</v>
+        <v>Material Wise</v>
       </c>
       <c r="E21" t="str">
         <f>VLOOKUP(B21, nodes!A:B, 2)</f>
-        <v>GreenScreen</v>
+        <v>C2C</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
+      <c r="A22" s="7">
+        <v>17</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>VLOOKUP(A22, nodes!A:B, 2)</f>
-        <v>USA/ME Safer Chemicals</v>
+        <v>IC2 Database</v>
       </c>
       <c r="E22" t="str">
         <f>VLOOKUP(B22, nodes!A:B, 2)</f>
@@ -2299,69 +2443,63 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>21</v>
+      <c r="A23" s="7">
+        <v>17</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D23" t="str">
         <f>VLOOKUP(A23, nodes!A:B, 2)</f>
-        <v>USA/WA SB 5181</v>
+        <v>IC2 Database</v>
       </c>
       <c r="E23" t="str">
         <f>VLOOKUP(B23, nodes!A:B, 2)</f>
-        <v>GreenScreen</v>
+        <v>QCAT</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="D24" t="str">
         <f>VLOOKUP(A24, nodes!A:B, 2)</f>
-        <v>CA DTSC Alternatives Assessment Guidance</v>
+        <v>SUBSPORT</v>
       </c>
       <c r="E24" t="str">
         <f>VLOOKUP(B24, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25">
         <v>0</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="D25" t="str">
         <f>VLOOKUP(A25, nodes!A:B, 2)</f>
-        <v>IC2 AA Guide</v>
+        <v>ToxFMD DB</v>
       </c>
       <c r="E25" t="str">
         <f>VLOOKUP(B25, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B26">
         <v>0</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="D26" t="str">
         <f>VLOOKUP(A26, nodes!A:B, 2)</f>
-        <v>NRC Framework Guide</v>
+        <v>Marketplace</v>
       </c>
       <c r="E26" t="str">
         <f>VLOOKUP(B26, nodes!A:B, 2)</f>
@@ -2370,36 +2508,154 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="D27" t="str">
         <f>VLOOKUP(A27, nodes!A:B, 2)</f>
-        <v>BizNGO AA Protocol</v>
+        <v>WA PBDE Law</v>
       </c>
       <c r="E27" t="str">
         <f>VLOOKUP(B27, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B28">
         <v>0</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D28" t="str">
         <f>VLOOKUP(A28, nodes!A:B, 2)</f>
-        <v>QCAT</v>
+        <v>Maine SCCP</v>
       </c>
       <c r="E28" t="str">
         <f>VLOOKUP(B28, nodes!A:B, 2)</f>
+        <v>GreenScreen</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>23</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="str">
+        <f>VLOOKUP(A29, nodes!A:B, 2)</f>
+        <v>DTSC AA</v>
+      </c>
+      <c r="E29" t="str">
+        <f>VLOOKUP(B29, nodes!A:B, 2)</f>
+        <v>GreenScreen</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>24</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="str">
+        <f>VLOOKUP(A30, nodes!A:B, 2)</f>
+        <v>QCAT</v>
+      </c>
+      <c r="E30" t="str">
+        <f>VLOOKUP(B30, nodes!A:B, 2)</f>
+        <v>GreenScreen</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="str">
+        <f>VLOOKUP(A31, nodes!A:B, 2)</f>
+        <v>IC2 AA</v>
+      </c>
+      <c r="E31" t="str">
+        <f>VLOOKUP(B31, nodes!A:B, 2)</f>
+        <v>GreenScreen</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="str">
+        <f>VLOOKUP(A32, nodes!A:B, 2)</f>
+        <v>NRC AA</v>
+      </c>
+      <c r="E32" t="str">
+        <f>VLOOKUP(B32, nodes!A:B, 2)</f>
+        <v>GreenScreen</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="str">
+        <f>VLOOKUP(A33, nodes!A:B, 2)</f>
+        <v>BizNGO AA</v>
+      </c>
+      <c r="E33" t="str">
+        <f>VLOOKUP(B33, nodes!A:B, 2)</f>
+        <v>GreenScreen</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="str">
+        <f>VLOOKUP(A34, nodes!A:B, 2)</f>
+        <v>Levis</v>
+      </c>
+      <c r="E34" t="str">
+        <f>VLOOKUP(B34, nodes!A:B, 2)</f>
+        <v>GreenScreen</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>29</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="str">
+        <f>VLOOKUP(A35, nodes!A:B, 2)</f>
+        <v>ILFI LPC</v>
+      </c>
+      <c r="E35" t="str">
+        <f>VLOOKUP(B35, nodes!A:B, 2)</f>
         <v>GreenScreen</v>
       </c>
     </row>

</xml_diff>